<commit_message>
try to modify excel file.
</commit_message>
<xml_diff>
--- a/doc/everyday management.xlsx
+++ b/doc/everyday management.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="20295" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="2775" windowWidth="17100" windowHeight="6045"/>
   </bookViews>
   <sheets>
     <sheet name="everyday" sheetId="1" r:id="rId1"/>
     <sheet name="绩效" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <r>
       <t>每天做了什么，有什么</t>
@@ -264,6 +265,10 @@
   </si>
   <si>
     <t>重写旧的服务器端代码、测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作时间也会成为绩效考核的一部分，虽然比例低，但是会考虑。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -655,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -706,6 +711,11 @@
     <row r="9" spans="1:1">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>